<commit_message>
working on data checks for dqo
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleDQOAccuracy_final.xlsx
+++ b/inst/extdata/ExampleDQOAccuracy_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbeck\R\win-library\4.1\MassWateR\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A00AE326-240C-4A2F-A9C3-349FC4FD9089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8781621D-0596-4FBF-A2D4-4AA3FBAD5081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31800" yWindow="2250" windowWidth="19455" windowHeight="9315" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="2460" yWindow="1572" windowWidth="19452" windowHeight="9312" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -51,21 +49,12 @@
     <t>Spike/Check Accuracy</t>
   </si>
   <si>
-    <t>Water Temp</t>
-  </si>
-  <si>
     <t>pH</t>
   </si>
   <si>
-    <t>DO</t>
-  </si>
-  <si>
     <t>± 5%</t>
   </si>
   <si>
-    <t>Conductivity</t>
-  </si>
-  <si>
     <t>TSS</t>
   </si>
   <si>
@@ -78,9 +67,6 @@
     <t>± 15%</t>
   </si>
   <si>
-    <t>ortho – P</t>
-  </si>
-  <si>
     <t>NO3</t>
   </si>
   <si>
@@ -88,9 +74,6 @@
   </si>
   <si>
     <t>Chloride</t>
-  </si>
-  <si>
-    <t>Chl-a</t>
   </si>
   <si>
     <t>uom</t>
@@ -216,9 +199,6 @@
     <t>UQL</t>
   </si>
   <si>
-    <t>E.coli</t>
-  </si>
-  <si>
     <t>cfu/100mL</t>
   </si>
   <si>
@@ -244,6 +224,24 @@
   </si>
   <si>
     <t>&lt;=log5%</t>
+  </si>
+  <si>
+    <t>E coli</t>
+  </si>
+  <si>
+    <t>chlorophyll a</t>
+  </si>
+  <si>
+    <t>orthoP</t>
+  </si>
+  <si>
+    <t>sp conductivity</t>
+  </si>
+  <si>
+    <t>DO concentration</t>
+  </si>
+  <si>
+    <t>water temperature</t>
   </si>
 </sst>
 </file>
@@ -679,7 +677,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,13 +693,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -713,10 +711,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>4</v>
@@ -724,520 +722,520 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7">
         <v>0.1</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7">
         <v>0.1</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7">
         <v>0.01</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7">
         <v>0.01</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="G11" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" s="7">
         <v>0.01</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C13" s="7">
         <v>0.01</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="7">
         <v>0.05</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C15" s="7">
         <v>0.05</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C17" s="7">
         <v>2</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C19" s="7">
         <v>10</v>
@@ -1246,30 +1244,30 @@
         <v>2400</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1278,30 +1276,30 @@
         <v>2400</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C21" s="7">
         <v>10</v>
@@ -1310,30 +1308,30 @@
         <v>2400</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C22" s="7">
         <v>10</v>
@@ -1342,22 +1340,22 @@
         <v>2400</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="G22" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added params mapping file and updated parameter names in results and dqo files to match #3
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleDQOAccuracy_final.xlsx
+++ b/inst/extdata/ExampleDQOAccuracy_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbeck\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8781621D-0596-4FBF-A2D4-4AA3FBAD5081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E168C-A129-4230-8ADA-C347D5ED5B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1572" windowWidth="19452" windowHeight="9312" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="2484" yWindow="2136" windowWidth="19452" windowHeight="9312" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>Parameter</t>
   </si>
@@ -49,10 +49,16 @@
     <t>Spike/Check Accuracy</t>
   </si>
   <si>
+    <t>Water Temp</t>
+  </si>
+  <si>
     <t>pH</t>
   </si>
   <si>
-    <t>± 5%</t>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
   </si>
   <si>
     <t>TSS</t>
@@ -62,9 +68,6 @@
   </si>
   <si>
     <t>TP</t>
-  </si>
-  <si>
-    <t>± 15%</t>
   </si>
   <si>
     <t>NO3</t>
@@ -151,21 +154,6 @@
     <t>&lt;= 30%</t>
   </si>
   <si>
-    <t>± 1</t>
-  </si>
-  <si>
-    <t>± 0.02</t>
-  </si>
-  <si>
-    <t>± 0.01</t>
-  </si>
-  <si>
-    <t>± 2</t>
-  </si>
-  <si>
-    <t>± 0.5</t>
-  </si>
-  <si>
     <t>&lt; 0.1</t>
   </si>
   <si>
@@ -175,12 +163,6 @@
     <t>&lt; 2</t>
   </si>
   <si>
-    <t>± 0.2</t>
-  </si>
-  <si>
-    <t>± 50</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -199,6 +181,9 @@
     <t>UQL</t>
   </si>
   <si>
+    <t>E.coli</t>
+  </si>
+  <si>
     <t>cfu/100mL</t>
   </si>
   <si>
@@ -226,22 +211,10 @@
     <t>&lt;=log5%</t>
   </si>
   <si>
-    <t>E coli</t>
-  </si>
-  <si>
-    <t>chlorophyll a</t>
-  </si>
-  <si>
-    <t>orthoP</t>
-  </si>
-  <si>
-    <t>sp conductivity</t>
-  </si>
-  <si>
-    <t>DO concentration</t>
-  </si>
-  <si>
-    <t>water temperature</t>
+    <t>Ortho P</t>
+  </si>
+  <si>
+    <t>Chl a</t>
   </si>
 </sst>
 </file>
@@ -334,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -357,6 +330,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,10 +650,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,13 +669,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -711,10 +687,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>4</v>
@@ -722,520 +698,520 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.5</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7">
         <v>0.1</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7">
         <v>0.1</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>6</v>
+        <v>37</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="J6" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="J7" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7">
         <v>0.01</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.01</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="7">
         <v>0.01</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7">
         <v>0.01</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.01</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="7">
         <v>0.01</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="7">
         <v>0.05</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="7">
         <v>0.05</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7">
         <v>2</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="I17" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C19" s="7">
         <v>10</v>
@@ -1244,30 +1220,30 @@
         <v>2400</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1276,30 +1252,30 @@
         <v>2400</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C21" s="7">
         <v>10</v>
@@ -1308,30 +1284,30 @@
         <v>2400</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7">
         <v>10</v>
@@ -1340,22 +1316,22 @@
         <v>2400</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added unit checks for check_dqoaccuracy #5
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleDQOAccuracy_final.xlsx
+++ b/inst/extdata/ExampleDQOAccuracy_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbeck\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E168C-A129-4230-8ADA-C347D5ED5B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C741A3F8-2AF2-46FE-A607-852B1DBEA3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2484" yWindow="2136" windowWidth="19452" windowHeight="9312" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="6915" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -70,12 +70,6 @@
     <t>TP</t>
   </si>
   <si>
-    <t>NO3</t>
-  </si>
-  <si>
-    <t>NH3</t>
-  </si>
-  <si>
     <t>Chloride</t>
   </si>
   <si>
@@ -85,36 +79,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>S.U.</t>
-  </si>
-  <si>
-    <t>mg/L</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S/cm</t>
-    </r>
-  </si>
-  <si>
-    <t>µg/L</t>
-  </si>
-  <si>
     <t>&lt; 4</t>
   </si>
   <si>
@@ -184,9 +148,6 @@
     <t>E.coli</t>
   </si>
   <si>
-    <t>cfu/100mL</t>
-  </si>
-  <si>
     <t>&lt;50</t>
   </si>
   <si>
@@ -215,6 +176,27 @@
   </si>
   <si>
     <t>Chl a</t>
+  </si>
+  <si>
+    <t>mg/l</t>
+  </si>
+  <si>
+    <t>uS/cm</t>
+  </si>
+  <si>
+    <t>s.u.</t>
+  </si>
+  <si>
+    <t>cfu/100ml</t>
+  </si>
+  <si>
+    <t>ug/l</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
   </si>
 </sst>
 </file>
@@ -650,32 +632,32 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="10" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -687,58 +669,58 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3" s="7">
         <v>0.5</v>
@@ -747,154 +729,154 @@
         <v>0.5</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J3" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7">
         <v>0.1</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J4" s="10">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7">
         <v>0.1</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J5" s="10">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J6" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J7" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>10</v>
@@ -903,52 +885,52 @@
         <v>10</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C10" s="7">
         <v>0.01</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7">
         <v>0.02</v>
@@ -966,55 +948,55 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7">
         <v>0.01</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J11" s="10">
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C12" s="7">
         <v>0.01</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F12" s="7">
         <v>0.01</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>10</v>
@@ -1026,115 +1008,115 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7">
         <v>0.01</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J13" s="10">
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C14" s="7">
         <v>0.05</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J14" s="10">
         <v>0.15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C15" s="7">
         <v>0.05</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J15" s="10">
         <v>0.15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>10</v>
@@ -1146,72 +1128,72 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C17" s="7">
         <v>2</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="B19" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
         <v>10</v>
@@ -1220,13 +1202,13 @@
         <v>2400</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>10</v>
@@ -1235,15 +1217,15 @@
         <v>10</v>
       </c>
       <c r="J19" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="B20" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1252,13 +1234,13 @@
         <v>2400</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>10</v>
@@ -1267,15 +1249,15 @@
         <v>10</v>
       </c>
       <c r="J20" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="B21" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7">
         <v>10</v>
@@ -1284,30 +1266,30 @@
         <v>2400</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C22" s="7">
         <v>10</v>
@@ -1316,13 +1298,13 @@
         <v>2400</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>10</v>
@@ -1331,7 +1313,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results file units for temp now deg C, removed formatting and checks that deal with degree symbols
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleDQOAccuracy_final.xlsx
+++ b/inst/extdata/ExampleDQOAccuracy_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C741A3F8-2AF2-46FE-A607-852B1DBEA3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DF923E-90AD-4C96-9078-F22C3F4CD968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="31980" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>uom</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>&lt; 4</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Ammonia</t>
+  </si>
+  <si>
+    <t>deg C</t>
   </si>
 </sst>
 </file>
@@ -632,10 +632,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,10 +654,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -669,10 +669,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>4</v>
@@ -683,29 +683,29 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -713,14 +713,14 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="7">
         <v>0.5</v>
@@ -729,10 +729,10 @@
         <v>0.5</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="7">
         <v>0.2</v>
@@ -743,26 +743,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7">
         <v>0.1</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="10">
         <v>0.05</v>
@@ -773,26 +773,26 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7">
         <v>0.1</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="10">
         <v>0.05</v>
@@ -803,26 +803,26 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="7">
         <v>50</v>
@@ -833,26 +833,26 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" s="7">
         <v>50</v>
@@ -863,20 +863,20 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>10</v>
@@ -885,7 +885,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -893,29 +893,29 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -923,14 +923,14 @@
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7">
         <v>0.01</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="7">
         <v>0.02</v>
@@ -953,26 +953,26 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="7">
         <v>0.01</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="10">
         <v>0.15</v>
@@ -980,23 +980,23 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="7">
         <v>0.01</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="7">
         <v>0.01</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>10</v>
@@ -1010,29 +1010,29 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="7">
         <v>0.01</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="10">
         <v>0.15</v>
@@ -1040,29 +1040,29 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="7">
         <v>0.05</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" s="10">
         <v>0.15</v>
@@ -1070,29 +1070,29 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7">
         <v>0.05</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J15" s="10">
         <v>0.15</v>
@@ -1103,20 +1103,20 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>10</v>
@@ -1130,70 +1130,70 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7">
         <v>2</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="7">
         <v>10</v>
@@ -1202,13 +1202,13 @@
         <v>2400</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>10</v>
@@ -1217,15 +1217,15 @@
         <v>10</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1234,13 +1234,13 @@
         <v>2400</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>10</v>
@@ -1249,15 +1249,15 @@
         <v>10</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7">
         <v>10</v>
@@ -1266,13 +1266,13 @@
         <v>2400</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>10</v>
@@ -1281,15 +1281,15 @@
         <v>10</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7">
         <v>10</v>
@@ -1298,13 +1298,13 @@
         <v>2400</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>10</v>
@@ -1313,7 +1313,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>